<commit_message>
Complete basic frontend setup
</commit_message>
<xml_diff>
--- a/reports/employee_safety.xlsx
+++ b/reports/employee_safety.xlsx
@@ -485,7 +485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -592,10 +592,94 @@
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t>2026-02-27 20:32:50</t>
+          <t>2026-02-27 23:07:03</t>
         </is>
       </c>
       <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>Missing PPE: Helmet, Safety Vest</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="22" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>EMP-003</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Sujal Ashok Vaidya</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Manufacturing</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>✗</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>✗</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>NOT READY</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>2026-02-27 23:06:38</t>
+        </is>
+      </c>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>Missing PPE: Helmet, Safety Vest</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="22" customHeight="1">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>EMP-004</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Vaibhav Hujaratti</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Electrical</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>✗</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>✗</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>NOT READY</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>2026-02-27 23:06:52</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
         <is>
           <t>Missing PPE: Helmet, Safety Vest</t>
         </is>

</xml_diff>